<commit_message>
Finish Primary V0.3 and Ambient V0.2
</commit_message>
<xml_diff>
--- a/SUMR25_River_Rockfish_Proj/Raw_Data/River's_Rockfish_Metadata_Parturition_V7.xlsx
+++ b/SUMR25_River_Rockfish_Proj/Raw_Data/River's_Rockfish_Metadata_Parturition_V7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmcke\OneDrive\Documents\Summer_2025_Rockfish_Research_Project\Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D524A6B-1E96-4562-A347-CAC68C934330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612F74E5-5198-4373-B56B-180B81EA4792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{1F309CE8-D94F-4E95-9E51-ED88FCC75EAC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="509">
   <si>
     <t>FISH_ID</t>
   </si>
@@ -5833,6 +5833,9 @@
   </si>
   <si>
     <t>All_Fecundity</t>
+  </si>
+  <si>
+    <t>Weight_Adj_Fec_With_Ateresia_Zeros</t>
   </si>
 </sst>
 </file>
@@ -6850,11 +6853,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98266282-F063-447E-BEE6-F317894BF3C6}">
-  <dimension ref="A1:BB68"/>
+  <dimension ref="A1:BC68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL4" sqref="AL4"/>
+      <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AZ36" sqref="AZ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6907,12 +6910,13 @@
     <col min="50" max="50" width="47" customWidth="1"/>
     <col min="51" max="51" width="21" customWidth="1"/>
     <col min="52" max="52" width="43.81640625" style="42" customWidth="1"/>
-    <col min="53" max="53" width="41.26953125" style="43" customWidth="1"/>
-    <col min="54" max="54" width="40.26953125" style="44" customWidth="1"/>
-    <col min="55" max="55" width="21.08984375" customWidth="1"/>
+    <col min="53" max="53" width="43.81640625" style="30" customWidth="1"/>
+    <col min="54" max="54" width="41.26953125" style="43" customWidth="1"/>
+    <col min="55" max="55" width="40.26953125" style="44" customWidth="1"/>
+    <col min="56" max="56" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -7069,14 +7073,17 @@
       <c r="AZ1" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="BA1" s="43" t="s">
+      <c r="BA1" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="BB1" s="43" t="s">
         <v>322</v>
       </c>
-      <c r="BB1" s="44" t="s">
+      <c r="BC1" s="44" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -7222,8 +7229,11 @@
       <c r="AZ2" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA2" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:55">
       <c r="A3" s="2">
         <v>97828</v>
       </c>
@@ -7368,8 +7378,11 @@
       <c r="AZ3" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA3" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:55">
       <c r="A4" s="2">
         <v>97811</v>
       </c>
@@ -7508,8 +7521,11 @@
       <c r="AZ4" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA4" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:55">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
@@ -7655,8 +7671,11 @@
         <f t="shared" ref="AZ5:AZ35" si="0">AJ5/AN5</f>
         <v>113.8416472007722</v>
       </c>
+      <c r="BA5" s="30">
+        <v>113.8416472007722</v>
+      </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -7804,8 +7823,11 @@
       <c r="AZ6" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA6" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:55">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -7948,8 +7970,11 @@
       <c r="AZ7" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA7" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:55">
       <c r="A8" s="2">
         <v>97838</v>
       </c>
@@ -8100,8 +8125,11 @@
       <c r="AZ8" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA8" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="9" spans="1:54">
+    <row r="9" spans="1:55">
       <c r="A9" s="2">
         <v>97812</v>
       </c>
@@ -8244,8 +8272,11 @@
         <f t="shared" si="0"/>
         <v>68.791115581232489</v>
       </c>
+      <c r="BA9" s="30">
+        <v>68.791115581232489</v>
+      </c>
     </row>
-    <row r="10" spans="1:54">
+    <row r="10" spans="1:55">
       <c r="A10" s="2">
         <v>97843</v>
       </c>
@@ -8394,8 +8425,11 @@
         <f t="shared" si="0"/>
         <v>271.558157999206</v>
       </c>
+      <c r="BA10" s="30">
+        <v>271.558157999206</v>
+      </c>
     </row>
-    <row r="11" spans="1:54">
+    <row r="11" spans="1:55">
       <c r="A11" s="2">
         <v>97833</v>
       </c>
@@ -8550,8 +8584,11 @@
         <f t="shared" si="0"/>
         <v>208.14822864594652</v>
       </c>
+      <c r="BA11" s="30">
+        <v>208.14822864594652</v>
+      </c>
     </row>
-    <row r="12" spans="1:54" s="61" customFormat="1">
+    <row r="12" spans="1:55" s="61" customFormat="1">
       <c r="A12" s="60" t="s">
         <v>51</v>
       </c>
@@ -8702,8 +8739,11 @@
       <c r="AZ12" s="61" t="s">
         <v>104</v>
       </c>
+      <c r="BA12" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="13" spans="1:54">
+    <row r="13" spans="1:55">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
@@ -8857,8 +8897,11 @@
       <c r="AZ13" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA13" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="14" spans="1:54">
+    <row r="14" spans="1:55">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -9007,8 +9050,11 @@
       <c r="AZ14" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA14" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="15" spans="1:54" s="61" customFormat="1">
+    <row r="15" spans="1:55" s="61" customFormat="1">
       <c r="A15" s="60" t="s">
         <v>54</v>
       </c>
@@ -9160,8 +9206,11 @@
         <f t="shared" si="0"/>
         <v>257.01186717758986</v>
       </c>
+      <c r="BA15" s="30">
+        <v>257.01186717758986</v>
+      </c>
     </row>
-    <row r="16" spans="1:54">
+    <row r="16" spans="1:55">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -9310,8 +9359,11 @@
         <f t="shared" si="0"/>
         <v>114.2072882158069</v>
       </c>
+      <c r="BA16" s="30">
+        <v>114.2072882158069</v>
+      </c>
     </row>
-    <row r="17" spans="1:52">
+    <row r="17" spans="1:53">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -9454,8 +9506,11 @@
         <f t="shared" si="0"/>
         <v>203.86814225713371</v>
       </c>
+      <c r="BA17" s="30">
+        <v>203.86814225713371</v>
+      </c>
     </row>
-    <row r="18" spans="1:52">
+    <row r="18" spans="1:53">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -9609,8 +9664,11 @@
       <c r="AZ18" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA18" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="19" spans="1:52">
+    <row r="19" spans="1:53">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -9761,8 +9819,11 @@
       <c r="AZ19" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA19" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:52">
+    <row r="20" spans="1:53">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
@@ -9916,8 +9977,11 @@
       <c r="AZ20" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA20" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="21" spans="1:52">
+    <row r="21" spans="1:53">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -10057,8 +10121,11 @@
         <f t="shared" si="0"/>
         <v>161.05197634609399</v>
       </c>
+      <c r="BA21" s="30">
+        <v>161.05197634609399</v>
+      </c>
     </row>
-    <row r="22" spans="1:52">
+    <row r="22" spans="1:53">
       <c r="A22" s="2" t="s">
         <v>61</v>
       </c>
@@ -10201,8 +10268,11 @@
         <f t="shared" si="0"/>
         <v>355.7167202937249</v>
       </c>
+      <c r="BA22" s="30">
+        <v>355.7167202937249</v>
+      </c>
     </row>
-    <row r="23" spans="1:52" s="61" customFormat="1">
+    <row r="23" spans="1:53" s="61" customFormat="1">
       <c r="A23" s="60" t="s">
         <v>62</v>
       </c>
@@ -10357,8 +10427,11 @@
         <f t="shared" si="0"/>
         <v>165.54735720638772</v>
       </c>
+      <c r="BA23" s="30">
+        <v>165.54735720638772</v>
+      </c>
     </row>
-    <row r="24" spans="1:52">
+    <row r="24" spans="1:53">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -10498,8 +10571,11 @@
         <f t="shared" si="0"/>
         <v>6.2158354466046779</v>
       </c>
+      <c r="BA24" s="30">
+        <v>6.2158354466046779</v>
+      </c>
     </row>
-    <row r="25" spans="1:52">
+    <row r="25" spans="1:53">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -10650,8 +10726,11 @@
       <c r="AZ25" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA25" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="26" spans="1:52">
+    <row r="26" spans="1:53">
       <c r="A26" s="2" t="s">
         <v>65</v>
       </c>
@@ -10791,8 +10870,11 @@
         <f t="shared" si="0"/>
         <v>147.56135934550031</v>
       </c>
+      <c r="BA26" s="30">
+        <v>147.56135934550031</v>
+      </c>
     </row>
-    <row r="27" spans="1:52">
+    <row r="27" spans="1:53">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -10943,8 +11025,11 @@
       <c r="AZ27" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA27" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="28" spans="1:52">
+    <row r="28" spans="1:53">
       <c r="A28" s="2">
         <v>77795</v>
       </c>
@@ -11087,8 +11172,11 @@
         <f t="shared" si="0"/>
         <v>180.71039999999999</v>
       </c>
+      <c r="BA28" s="30">
+        <v>180.71039999999999</v>
+      </c>
     </row>
-    <row r="29" spans="1:52">
+    <row r="29" spans="1:53">
       <c r="A29" s="2" t="s">
         <v>67</v>
       </c>
@@ -11228,8 +11316,11 @@
         <f t="shared" si="0"/>
         <v>241.89097103918229</v>
       </c>
+      <c r="BA29" s="30">
+        <v>241.89097103918229</v>
+      </c>
     </row>
-    <row r="30" spans="1:52">
+    <row r="30" spans="1:53">
       <c r="A30" s="2" t="s">
         <v>68</v>
       </c>
@@ -11369,8 +11460,11 @@
         <f t="shared" si="0"/>
         <v>222.42606854866645</v>
       </c>
+      <c r="BA30" s="30">
+        <v>222.42606854866645</v>
+      </c>
     </row>
-    <row r="31" spans="1:52" s="61" customFormat="1">
+    <row r="31" spans="1:53" s="61" customFormat="1">
       <c r="A31" s="60" t="s">
         <v>69</v>
       </c>
@@ -11522,8 +11616,11 @@
         <f t="shared" si="0"/>
         <v>1.4217727543129091</v>
       </c>
+      <c r="BA31" s="30">
+        <v>1.4217727543129091</v>
+      </c>
     </row>
-    <row r="32" spans="1:52">
+    <row r="32" spans="1:53">
       <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
@@ -11666,8 +11763,11 @@
         <f t="shared" si="0"/>
         <v>77.660757733750444</v>
       </c>
+      <c r="BA32" s="30">
+        <v>77.660757733750444</v>
+      </c>
     </row>
-    <row r="33" spans="1:52">
+    <row r="33" spans="1:53">
       <c r="A33" s="2" t="s">
         <v>71</v>
       </c>
@@ -11810,8 +11910,11 @@
         <f t="shared" si="0"/>
         <v>337.64382424577911</v>
       </c>
+      <c r="BA33" s="30">
+        <v>337.64382424577911</v>
+      </c>
     </row>
-    <row r="34" spans="1:52">
+    <row r="34" spans="1:53">
       <c r="A34" s="2" t="s">
         <v>72</v>
       </c>
@@ -11954,8 +12057,11 @@
         <f t="shared" si="0"/>
         <v>25.779702970297031</v>
       </c>
+      <c r="BA34" s="30">
+        <v>25.779702970297031</v>
+      </c>
     </row>
-    <row r="35" spans="1:52">
+    <row r="35" spans="1:53">
       <c r="A35" s="2" t="s">
         <v>73</v>
       </c>
@@ -12098,8 +12204,11 @@
         <f t="shared" si="0"/>
         <v>93.575337468077336</v>
       </c>
+      <c r="BA35" s="30">
+        <v>93.575337468077336</v>
+      </c>
     </row>
-    <row r="36" spans="1:52">
+    <row r="36" spans="1:53">
       <c r="A36" s="2">
         <v>97824</v>
       </c>
@@ -12253,8 +12362,11 @@
       <c r="AZ36" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA36" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:52">
+    <row r="37" spans="1:53">
       <c r="A37" s="2">
         <v>97827</v>
       </c>
@@ -12408,8 +12520,11 @@
       <c r="AZ37" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA37" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:52">
+    <row r="38" spans="1:53">
       <c r="A38" s="1" t="s">
         <v>252</v>
       </c>
@@ -12560,8 +12675,11 @@
       <c r="AZ38" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA38" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:52">
+    <row r="39" spans="1:53">
       <c r="A39" s="2" t="s">
         <v>254</v>
       </c>
@@ -12712,8 +12830,11 @@
       <c r="AZ39" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA39" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:52">
+    <row r="40" spans="1:53">
       <c r="A40" s="2">
         <v>97830</v>
       </c>
@@ -12867,8 +12988,11 @@
       <c r="AZ40" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA40" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:52">
+    <row r="41" spans="1:53">
       <c r="A41" s="2">
         <v>97823</v>
       </c>
@@ -13019,8 +13143,11 @@
       <c r="AZ41" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA41" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:52">
+    <row r="42" spans="1:53">
       <c r="A42" s="2">
         <v>97836</v>
       </c>
@@ -13174,8 +13301,11 @@
       <c r="AZ42" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA42" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:52">
+    <row r="43" spans="1:53">
       <c r="A43" s="1" t="s">
         <v>259</v>
       </c>
@@ -13329,8 +13459,11 @@
       <c r="AZ43" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA43" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:52">
+    <row r="44" spans="1:53">
       <c r="A44" s="2">
         <v>97822</v>
       </c>
@@ -13484,8 +13617,11 @@
       <c r="AZ44" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA44" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:52">
+    <row r="45" spans="1:53">
       <c r="A45" s="1" t="s">
         <v>264</v>
       </c>
@@ -13636,8 +13772,11 @@
       <c r="AZ45" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA45" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:52">
+    <row r="46" spans="1:53">
       <c r="A46" s="1" t="s">
         <v>267</v>
       </c>
@@ -13791,8 +13930,11 @@
       <c r="AZ46" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA46" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:52">
+    <row r="47" spans="1:53">
       <c r="A47" s="2">
         <v>97805</v>
       </c>
@@ -13949,8 +14091,11 @@
       <c r="AZ47" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA47" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:52">
+    <row r="48" spans="1:53">
       <c r="A48" s="1" t="s">
         <v>273</v>
       </c>
@@ -14101,8 +14246,11 @@
       <c r="AZ48" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA48" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:52">
+    <row r="49" spans="1:53">
       <c r="A49" s="2">
         <v>97841</v>
       </c>
@@ -14253,8 +14401,11 @@
       <c r="AZ49" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA49" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:52">
+    <row r="50" spans="1:53">
       <c r="A50" s="2">
         <v>97825</v>
       </c>
@@ -14408,8 +14559,11 @@
       <c r="AZ50" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA50" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:52">
+    <row r="51" spans="1:53">
       <c r="A51" s="1" t="s">
         <v>281</v>
       </c>
@@ -14560,8 +14714,11 @@
       <c r="AZ51" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA51" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:52">
+    <row r="52" spans="1:53">
       <c r="A52" s="1" t="s">
         <v>283</v>
       </c>
@@ -14712,8 +14869,11 @@
       <c r="AZ52" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA52" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:52">
+    <row r="53" spans="1:53">
       <c r="A53" s="2">
         <v>97801</v>
       </c>
@@ -14867,8 +15027,11 @@
       <c r="AZ53" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA53" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:52">
+    <row r="54" spans="1:53">
       <c r="A54" s="1" t="s">
         <v>288</v>
       </c>
@@ -15022,8 +15185,11 @@
       <c r="AZ54" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA54" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:52">
+    <row r="55" spans="1:53">
       <c r="A55" s="2">
         <v>97816</v>
       </c>
@@ -15180,8 +15346,11 @@
       <c r="AZ55" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA55" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:52">
+    <row r="56" spans="1:53">
       <c r="A56" s="1" t="s">
         <v>293</v>
       </c>
@@ -15335,8 +15504,11 @@
       <c r="AZ56" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA56" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:52">
+    <row r="57" spans="1:53">
       <c r="A57" s="2">
         <v>97808</v>
       </c>
@@ -15490,8 +15662,11 @@
       <c r="AZ57" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA57" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:52">
+    <row r="58" spans="1:53">
       <c r="A58" s="1" t="s">
         <v>300</v>
       </c>
@@ -15645,8 +15820,11 @@
       <c r="AZ58" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA58" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:52">
+    <row r="59" spans="1:53">
       <c r="A59" s="1" t="s">
         <v>302</v>
       </c>
@@ -15800,8 +15978,11 @@
       <c r="AZ59" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA59" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:52">
+    <row r="60" spans="1:53">
       <c r="A60" s="40">
         <v>97821</v>
       </c>
@@ -15952,8 +16133,11 @@
       <c r="AZ60" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA60" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:52">
+    <row r="61" spans="1:53">
       <c r="A61" s="2">
         <v>97807</v>
       </c>
@@ -16107,8 +16291,11 @@
       <c r="AZ61" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA61" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:52">
+    <row r="62" spans="1:53">
       <c r="A62" s="2">
         <v>97706</v>
       </c>
@@ -16169,8 +16356,11 @@
       <c r="AZ62" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA62" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="63" spans="1:52">
+    <row r="63" spans="1:53">
       <c r="A63" s="1" t="s">
         <v>309</v>
       </c>
@@ -16324,8 +16514,11 @@
       <c r="AZ63" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA63" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:52">
+    <row r="64" spans="1:53">
       <c r="A64" s="2">
         <v>97844</v>
       </c>
@@ -16479,8 +16672,11 @@
       <c r="AZ64" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA64" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:52">
+    <row r="65" spans="1:53">
       <c r="A65" s="2">
         <v>97820</v>
       </c>
@@ -16631,8 +16827,11 @@
       <c r="AZ65" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA65" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:52">
+    <row r="66" spans="1:53">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -16786,8 +16985,11 @@
       <c r="AZ66" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA66" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:52">
+    <row r="67" spans="1:53">
       <c r="A67" s="2">
         <v>97803</v>
       </c>
@@ -16938,8 +17140,11 @@
       <c r="AZ67" s="42" t="s">
         <v>104</v>
       </c>
+      <c r="BA67" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:52">
+    <row r="68" spans="1:53">
       <c r="A68" s="2">
         <v>97831</v>
       </c>
@@ -17092,6 +17297,9 @@
       </c>
       <c r="AZ68" s="42" t="s">
         <v>104</v>
+      </c>
+      <c r="BA68" s="30">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>